<commit_message>
added some of the battle logic changed type enums
</commit_message>
<xml_diff>
--- a/docs/MTCG_workLog.xlsx
+++ b/docs/MTCG_workLog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\varga\source\repos\MTCG-WS2023\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DE1BD89-4567-4412-8A37-832C8F445290}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{941BE4C4-BB65-440D-9D4D-5F9C58ABE6DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{5680B013-B747-48BE-B841-37A06F1D94CC}"/>
+    <workbookView xWindow="2688" yWindow="3288" windowWidth="17280" windowHeight="8964" xr2:uid="{5680B013-B747-48BE-B841-37A06F1D94CC}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>Date</t>
   </si>
@@ -63,6 +63,15 @@
   </si>
   <si>
     <t>18:50-19:40</t>
+  </si>
+  <si>
+    <t>12:20-15:45</t>
+  </si>
+  <si>
+    <t>01.11.2023</t>
+  </si>
+  <si>
+    <t>Getting started on coding</t>
   </si>
 </sst>
 </file>
@@ -422,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21265F0A-4FFE-4DCE-A935-735B58544DF9}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -471,6 +480,17 @@
         <v>5</v>
       </c>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
start on server logic
</commit_message>
<xml_diff>
--- a/docs/MTCG_workLog.xlsx
+++ b/docs/MTCG_workLog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\varga\source\repos\MTCG-WS2023\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{941BE4C4-BB65-440D-9D4D-5F9C58ABE6DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE516ACE-7230-42D6-B87A-2776FA1FFB74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="3288" windowWidth="17280" windowHeight="8964" xr2:uid="{5680B013-B747-48BE-B841-37A06F1D94CC}"/>
+    <workbookView xWindow="1536" yWindow="2136" windowWidth="17280" windowHeight="8964" xr2:uid="{5680B013-B747-48BE-B841-37A06F1D94CC}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,14 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>Date</t>
   </si>
   <si>
-    <t>Time</t>
-  </si>
-  <si>
     <t>Work description</t>
   </si>
   <si>
@@ -72,6 +69,33 @@
   </si>
   <si>
     <t>Getting started on coding</t>
+  </si>
+  <si>
+    <t>13:00-15:30</t>
+  </si>
+  <si>
+    <t>06.11.2023</t>
+  </si>
+  <si>
+    <t>Worked on battle logic</t>
+  </si>
+  <si>
+    <t>Time (in minutes)</t>
+  </si>
+  <si>
+    <t>Temp Hour counter</t>
+  </si>
+  <si>
+    <t>08.12.2023</t>
+  </si>
+  <si>
+    <t>Got started on HTTP Server</t>
+  </si>
+  <si>
+    <t>15:30-20:00</t>
+  </si>
+  <si>
+    <t>13:30-zeit</t>
   </si>
 </sst>
 </file>
@@ -431,64 +455,115 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21265F0A-4FFE-4DCE-A935-735B58544DF9}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="57.109375" customWidth="1"/>
     <col min="4" max="4" width="35" customWidth="1"/>
+    <col min="6" max="6" width="16.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="B2">
+        <v>50</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2">
+        <f>SUM(B2:B250)/60</f>
+        <v>11.75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>30</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="2" t="s">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <v>205</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5">
+        <v>150</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D4" t="s">
-        <v>9</v>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6">
+        <v>270</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D7" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
got started on db + "experimentation" with interface for creating tables (idea will probably be scrapped)
</commit_message>
<xml_diff>
--- a/docs/MTCG_workLog.xlsx
+++ b/docs/MTCG_workLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\varga\source\repos\MTCG-WS2023\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE516ACE-7230-42D6-B87A-2776FA1FFB74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFC5E708-3634-4DD6-BA39-9020ADD10BCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1536" yWindow="2136" windowWidth="17280" windowHeight="8964" xr2:uid="{5680B013-B747-48BE-B841-37A06F1D94CC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
   <si>
     <t>Date</t>
   </si>
@@ -95,7 +95,28 @@
     <t>15:30-20:00</t>
   </si>
   <si>
-    <t>13:30-zeit</t>
+    <t>13:30-20:00</t>
+  </si>
+  <si>
+    <t>13.12.2023</t>
+  </si>
+  <si>
+    <t>Continued on Server</t>
+  </si>
+  <si>
+    <t>12.12.2023</t>
+  </si>
+  <si>
+    <t>18:30-20:00</t>
+  </si>
+  <si>
+    <t>18.12.2023</t>
+  </si>
+  <si>
+    <t>Started on DB</t>
+  </si>
+  <si>
+    <t>15:30-19:00</t>
   </si>
 </sst>
 </file>
@@ -455,10 +476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21265F0A-4FFE-4DCE-A935-735B58544DF9}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -502,7 +523,7 @@
       </c>
       <c r="F2">
         <f>SUM(B2:B250)/60</f>
-        <v>11.75</v>
+        <v>23.25</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -562,8 +583,45 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7">
+        <v>390</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
       <c r="D7" s="2" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8">
+        <v>90</v>
+      </c>
+      <c r="C8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9">
+        <v>210</v>
+      </c>
+      <c r="C9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finished inital database setup + got started on request handling
</commit_message>
<xml_diff>
--- a/docs/MTCG_workLog.xlsx
+++ b/docs/MTCG_workLog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\varga\source\repos\MTCG-WS2023\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFC5E708-3634-4DD6-BA39-9020ADD10BCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8407D828-6FF6-4FAA-928D-14AB563F25CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="2136" windowWidth="17280" windowHeight="8964" xr2:uid="{5680B013-B747-48BE-B841-37A06F1D94CC}"/>
+    <workbookView xWindow="1920" yWindow="2520" windowWidth="17280" windowHeight="8964" xr2:uid="{5680B013-B747-48BE-B841-37A06F1D94CC}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
   <si>
     <t>Date</t>
   </si>
@@ -117,6 +117,15 @@
   </si>
   <si>
     <t>15:30-19:00</t>
+  </si>
+  <si>
+    <t>19.12.2023</t>
+  </si>
+  <si>
+    <t>13:00-15:00; 16:00-20:00</t>
+  </si>
+  <si>
+    <t>DB + request handling start</t>
   </si>
 </sst>
 </file>
@@ -476,10 +485,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21265F0A-4FFE-4DCE-A935-735B58544DF9}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -523,7 +532,7 @@
       </c>
       <c r="F2">
         <f>SUM(B2:B250)/60</f>
-        <v>23.25</v>
+        <v>29.25</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -622,6 +631,20 @@
       </c>
       <c r="D9" s="2" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10">
+        <v>360</v>
+      </c>
+      <c r="C10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
converted server and dbManager to singletons; got started on PostUser implementation; added schemas folder
</commit_message>
<xml_diff>
--- a/docs/MTCG_workLog.xlsx
+++ b/docs/MTCG_workLog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\varga\source\repos\MTCG-WS2023\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8407D828-6FF6-4FAA-928D-14AB563F25CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C137EF5F-6E1E-4AAE-AE10-C2E83E7B25C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="2520" windowWidth="17280" windowHeight="8964" xr2:uid="{5680B013-B747-48BE-B841-37A06F1D94CC}"/>
+    <workbookView xWindow="1536" yWindow="2136" windowWidth="17280" windowHeight="8964" xr2:uid="{5680B013-B747-48BE-B841-37A06F1D94CC}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
   <si>
     <t>Date</t>
   </si>
@@ -126,6 +126,12 @@
   </si>
   <si>
     <t>DB + request handling start</t>
+  </si>
+  <si>
+    <t>13:00-zeit</t>
+  </si>
+  <si>
+    <t>22.12.2023</t>
   </si>
 </sst>
 </file>
@@ -485,10 +491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21265F0A-4FFE-4DCE-A935-735B58544DF9}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -647,6 +653,14 @@
         <v>28</v>
       </c>
     </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
PostUser implemented + working :D + added all httprequest classes
</commit_message>
<xml_diff>
--- a/docs/MTCG_workLog.xlsx
+++ b/docs/MTCG_workLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\varga\source\repos\MTCG-WS2023\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C137EF5F-6E1E-4AAE-AE10-C2E83E7B25C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{906B3ED5-4536-4DF3-9B81-E3BC957C465E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1536" yWindow="2136" windowWidth="17280" windowHeight="8964" xr2:uid="{5680B013-B747-48BE-B841-37A06F1D94CC}"/>
   </bookViews>
@@ -128,10 +128,10 @@
     <t>DB + request handling start</t>
   </si>
   <si>
-    <t>13:00-zeit</t>
-  </si>
-  <si>
     <t>22.12.2023</t>
+  </si>
+  <si>
+    <t>13:00-15:00; 16:30-</t>
   </si>
 </sst>
 </file>
@@ -494,7 +494,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -655,10 +655,10 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
created all db schemas
</commit_message>
<xml_diff>
--- a/docs/MTCG_workLog.xlsx
+++ b/docs/MTCG_workLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\varga\source\repos\MTCG-WS2023\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{906B3ED5-4536-4DF3-9B81-E3BC957C465E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9942077F-A060-4F10-A876-54D4E145080D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1536" yWindow="2136" windowWidth="17280" windowHeight="8964" xr2:uid="{5680B013-B747-48BE-B841-37A06F1D94CC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
   <si>
     <t>Date</t>
   </si>
@@ -131,7 +131,10 @@
     <t>22.12.2023</t>
   </si>
   <si>
-    <t>13:00-15:00; 16:30-</t>
+    <t>13:00-15:00; 16:30-18:30</t>
+  </si>
+  <si>
+    <t>Implemented PostUser; made server/dbManager singleton/misc.</t>
   </si>
 </sst>
 </file>
@@ -494,7 +497,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -538,7 +541,7 @@
       </c>
       <c r="F2">
         <f>SUM(B2:B250)/60</f>
-        <v>29.25</v>
+        <v>33.25</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -656,6 +659,12 @@
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>30</v>
+      </c>
+      <c r="B11">
+        <v>240</v>
+      </c>
+      <c r="C11" t="s">
+        <v>32</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
PostPackage (creating packages) implemented
</commit_message>
<xml_diff>
--- a/docs/MTCG_workLog.xlsx
+++ b/docs/MTCG_workLog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\varga\source\repos\MTCG-WS2023\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9942077F-A060-4F10-A876-54D4E145080D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B8EDD1E-62C9-45EB-8038-CF2E09DA4206}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="2136" windowWidth="17280" windowHeight="8964" xr2:uid="{5680B013-B747-48BE-B841-37A06F1D94CC}"/>
+    <workbookView xWindow="2688" yWindow="3288" windowWidth="17280" windowHeight="8964" xr2:uid="{5680B013-B747-48BE-B841-37A06F1D94CC}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
   <si>
     <t>Date</t>
   </si>
@@ -135,6 +135,12 @@
   </si>
   <si>
     <t>Implemented PostUser; made server/dbManager singleton/misc.</t>
+  </si>
+  <si>
+    <t>13:30-zeit</t>
+  </si>
+  <si>
+    <t>27.12.2023</t>
   </si>
 </sst>
 </file>
@@ -494,10 +500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21265F0A-4FFE-4DCE-A935-735B58544DF9}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -670,6 +676,14 @@
         <v>31</v>
       </c>
     </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
divided users table into 3 tables; updated PostUser todo: update GetUser, update PutUser
</commit_message>
<xml_diff>
--- a/docs/MTCG_workLog.xlsx
+++ b/docs/MTCG_workLog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\varga\source\repos\MTCG-WS2023\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90E897E9-097D-4511-9E7A-3399B7ABA6F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54927DAB-8891-496C-9EA2-9A03D9417A4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3705" yWindow="4935" windowWidth="17280" windowHeight="8970" xr2:uid="{5680B013-B747-48BE-B841-37A06F1D94CC}"/>
+    <workbookView xWindow="2304" yWindow="2904" windowWidth="17280" windowHeight="8964" xr2:uid="{5680B013-B747-48BE-B841-37A06F1D94CC}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="44">
   <si>
     <t>Date</t>
   </si>
@@ -156,6 +156,18 @@
   </si>
   <si>
     <t>12:00-17:00</t>
+  </si>
+  <si>
+    <t>21:00-23:15</t>
+  </si>
+  <si>
+    <t>01.01.2024</t>
+  </si>
+  <si>
+    <t>02.01.2023</t>
+  </si>
+  <si>
+    <t>12:40-zeit</t>
   </si>
 </sst>
 </file>
@@ -515,22 +527,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21265F0A-4FFE-4DCE-A935-735B58544DF9}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="57.140625" customWidth="1"/>
+    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="57.109375" customWidth="1"/>
     <col min="4" max="4" width="35" customWidth="1"/>
-    <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -547,7 +559,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -562,10 +574,10 @@
       </c>
       <c r="F2">
         <f>SUM(B2:B250)/60</f>
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>56.25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -579,7 +591,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -593,7 +605,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -607,7 +619,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -621,7 +633,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -635,7 +647,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -649,7 +661,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -663,7 +675,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -677,7 +689,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -691,7 +703,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -705,7 +717,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -719,7 +731,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>38</v>
       </c>
@@ -731,6 +743,31 @@
       </c>
       <c r="D14" s="2" t="s">
         <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15">
+        <v>135</v>
+      </c>
+      <c r="C15" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
trading complete !!! hihihihi
</commit_message>
<xml_diff>
--- a/docs/MTCG_workLog.xlsx
+++ b/docs/MTCG_workLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\varga\source\repos\MTCG-WS2023\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F16731A-C61B-4578-A35B-56315E5990E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67912058-7D0C-4346-991A-11BCB3DCC664}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1920" yWindow="2520" windowWidth="17280" windowHeight="8964" xr2:uid="{5680B013-B747-48BE-B841-37A06F1D94CC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="47">
   <si>
     <t>Date</t>
   </si>
@@ -173,7 +173,10 @@
     <t>02.01.2024</t>
   </si>
   <si>
-    <t>i got sick :(</t>
+    <t>16:00-18:00; i got sick :(</t>
+  </si>
+  <si>
+    <t>11:00-zeit</t>
   </si>
 </sst>
 </file>
@@ -533,10 +536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21265F0A-4FFE-4DCE-A935-735B58544DF9}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -581,7 +584,7 @@
       </c>
       <c r="F2">
         <f>SUM(B2:B250)/60</f>
-        <v>63.75</v>
+        <v>65.75</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -784,8 +787,22 @@
       <c r="A17" t="s">
         <v>43</v>
       </c>
+      <c r="B17">
+        <v>120</v>
+      </c>
+      <c r="C17" t="s">
+        <v>37</v>
+      </c>
       <c r="D17" s="2" t="s">
         <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implemented card specialties + some fever dream code ??
</commit_message>
<xml_diff>
--- a/docs/MTCG_workLog.xlsx
+++ b/docs/MTCG_workLog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\varga\source\repos\MTCG-WS2023\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67912058-7D0C-4346-991A-11BCB3DCC664}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53FFB6A2-BF9C-43C6-9CC3-A5B8B7E3C081}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="2520" windowWidth="17280" windowHeight="8964" xr2:uid="{5680B013-B747-48BE-B841-37A06F1D94CC}"/>
+    <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{5680B013-B747-48BE-B841-37A06F1D94CC}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="51">
   <si>
     <t>Date</t>
   </si>
@@ -176,7 +176,19 @@
     <t>16:00-18:00; i got sick :(</t>
   </si>
   <si>
-    <t>11:00-zeit</t>
+    <t>finished all requests but battle</t>
+  </si>
+  <si>
+    <t>11:00-12:00; 13:30-15:50; still sick and it got worse TT-TT</t>
+  </si>
+  <si>
+    <t>04.01.2024</t>
+  </si>
+  <si>
+    <t>10:20-zeit</t>
+  </si>
+  <si>
+    <t>05.01.2024</t>
   </si>
 </sst>
 </file>
@@ -536,10 +548,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21265F0A-4FFE-4DCE-A935-735B58544DF9}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -547,7 +559,7 @@
     <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="57.109375" customWidth="1"/>
-    <col min="4" max="4" width="43.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.21875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.6640625" customWidth="1"/>
     <col min="6" max="6" width="16.88671875" bestFit="1" customWidth="1"/>
   </cols>
@@ -584,7 +596,7 @@
       </c>
       <c r="F2">
         <f>SUM(B2:B250)/60</f>
-        <v>65.75</v>
+        <v>69.083333333333329</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -799,10 +811,24 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>41</v>
+        <v>48</v>
+      </c>
+      <c r="B18">
+        <v>200</v>
+      </c>
+      <c r="C18" t="s">
+        <v>46</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>50</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
BATTLELOG GETS RETURNED TO BOTH PLAYERS !!!!! COMMITTING NOW IN CASE I FUCK SOMETHING UP AGAIN
</commit_message>
<xml_diff>
--- a/docs/MTCG_workLog.xlsx
+++ b/docs/MTCG_workLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\varga\source\repos\MTCG-WS2023\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53FFB6A2-BF9C-43C6-9CC3-A5B8B7E3C081}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9307E682-FF57-4277-9233-88537B10ACEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{5680B013-B747-48BE-B841-37A06F1D94CC}"/>
   </bookViews>
@@ -185,10 +185,10 @@
     <t>04.01.2024</t>
   </si>
   <si>
-    <t>10:20-zeit</t>
-  </si>
-  <si>
     <t>05.01.2024</t>
+  </si>
+  <si>
+    <t>10:20-14:40; 16:30-</t>
   </si>
 </sst>
 </file>
@@ -551,7 +551,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -825,10 +825,10 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>49</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
moved all postgresql statements into DataAccess class
</commit_message>
<xml_diff>
--- a/docs/MTCG_workLog.xlsx
+++ b/docs/MTCG_workLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\varga\source\repos\MTCG-WS2023\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{617E90D5-126C-45A1-B4CD-6C2DCC65CE4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D26DFBC4-9417-4512-B6ED-1E1610ED62CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{5680B013-B747-48BE-B841-37A06F1D94CC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="55">
   <si>
     <t>Date</t>
   </si>
@@ -188,10 +188,19 @@
     <t>05.01.2024</t>
   </si>
   <si>
-    <t>10:20-14:40; 16:30-18:30; 22:00-23:35</t>
-  </si>
-  <si>
     <t>finished battle &amp; mandatory unique feature (TODO: unittests, cleanup, protocol)</t>
+  </si>
+  <si>
+    <t>10:20-14:40; 16:30-18:30; 22:00-23:35; sickness shall not beat me</t>
+  </si>
+  <si>
+    <t>06.01.2024</t>
+  </si>
+  <si>
+    <t>14:40-22:30; 23:30-zeit</t>
+  </si>
+  <si>
+    <t>polishing (db layer)</t>
   </si>
 </sst>
 </file>
@@ -551,10 +560,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21265F0A-4FFE-4DCE-A935-735B58544DF9}">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -562,7 +571,7 @@
     <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="66.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="48.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="55.21875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.6640625" customWidth="1"/>
     <col min="6" max="6" width="16.88671875" bestFit="1" customWidth="1"/>
   </cols>
@@ -834,10 +843,21 @@
         <v>475</v>
       </c>
       <c r="C19" t="s">
+        <v>50</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>50</v>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" t="s">
+        <v>54</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
some unittests + can't add card to deck if engaged in trade
</commit_message>
<xml_diff>
--- a/docs/MTCG_workLog.xlsx
+++ b/docs/MTCG_workLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\varga\source\repos\MTCG-WS2023\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D26DFBC4-9417-4512-B6ED-1E1610ED62CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D230ED3-86AE-4CA7-88B4-D3B513FCBB9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{5680B013-B747-48BE-B841-37A06F1D94CC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="57">
   <si>
     <t>Date</t>
   </si>
@@ -197,10 +197,16 @@
     <t>06.01.2024</t>
   </si>
   <si>
-    <t>14:40-22:30; 23:30-zeit</t>
-  </si>
-  <si>
     <t>polishing (db layer)</t>
+  </si>
+  <si>
+    <t>14:40-22:30; 23:30-02:15</t>
+  </si>
+  <si>
+    <t>unit tests</t>
+  </si>
+  <si>
+    <t>10:30-12:00; 13:30-zeit</t>
   </si>
 </sst>
 </file>
@@ -560,10 +566,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21265F0A-4FFE-4DCE-A935-735B58544DF9}">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -854,10 +860,18 @@
         <v>52</v>
       </c>
       <c r="C20" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D20" s="2" t="s">
-        <v>53</v>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C21" t="s">
+        <v>55</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added GetDeckPlain + got started on protocol
</commit_message>
<xml_diff>
--- a/docs/MTCG_workLog.xlsx
+++ b/docs/MTCG_workLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\varga\source\repos\MTCG-WS2023\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D230ED3-86AE-4CA7-88B4-D3B513FCBB9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D192685C-C12C-4D49-B2FC-EC92DD4239FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{5680B013-B747-48BE-B841-37A06F1D94CC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="58">
   <si>
     <t>Date</t>
   </si>
@@ -203,10 +203,13 @@
     <t>14:40-22:30; 23:30-02:15</t>
   </si>
   <si>
-    <t>unit tests</t>
-  </si>
-  <si>
     <t>10:30-12:00; 13:30-zeit</t>
+  </si>
+  <si>
+    <t>unit tests, protocol</t>
+  </si>
+  <si>
+    <t>07.01.2024</t>
   </si>
 </sst>
 </file>
@@ -569,7 +572,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -614,7 +617,7 @@
       </c>
       <c r="F2">
         <f>SUM(B2:B250)/60</f>
-        <v>77</v>
+        <v>84.833333333333329</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -859,6 +862,9 @@
       <c r="A20" t="s">
         <v>52</v>
       </c>
+      <c r="B20">
+        <v>470</v>
+      </c>
       <c r="C20" t="s">
         <v>53</v>
       </c>
@@ -867,11 +873,14 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>57</v>
+      </c>
       <c r="C21" t="s">
+        <v>56</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
unit tests + final polishing
</commit_message>
<xml_diff>
--- a/docs/MTCG_workLog.xlsx
+++ b/docs/MTCG_workLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\varga\source\repos\MTCG-WS2023\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D192685C-C12C-4D49-B2FC-EC92DD4239FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52CE6955-74C9-47D4-8318-B47DB7597553}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{5680B013-B747-48BE-B841-37A06F1D94CC}"/>
   </bookViews>
@@ -203,13 +203,13 @@
     <t>14:40-22:30; 23:30-02:15</t>
   </si>
   <si>
-    <t>10:30-12:00; 13:30-zeit</t>
-  </si>
-  <si>
     <t>unit tests, protocol</t>
   </si>
   <si>
     <t>07.01.2024</t>
+  </si>
+  <si>
+    <t>10:30-12:00; 13:30-15:00;16:00:19:00;20:00-22:30</t>
   </si>
 </sst>
 </file>
@@ -572,7 +572,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -617,7 +617,7 @@
       </c>
       <c r="F2">
         <f>SUM(B2:B250)/60</f>
-        <v>84.833333333333329</v>
+        <v>93.333333333333329</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -874,13 +874,16 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21">
+        <v>510</v>
+      </c>
+      <c r="C21" t="s">
+        <v>55</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="C21" t="s">
-        <v>56</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>